<commit_message>
temp fix raw stock list
</commit_message>
<xml_diff>
--- a/.xlsx/current_total_stock_list.xlsx
+++ b/.xlsx/current_total_stock_list.xlsx
@@ -443,4319 +443,4319 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HND</t>
+          <t>PVM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>STK</t>
+          <t>LAS</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KDH</t>
+          <t>ADS</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ITC</t>
+          <t>LIX</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TMS</t>
+          <t>NLG</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PGB</t>
+          <t>VE9</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CMX</t>
+          <t>FOX</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MVC</t>
+          <t>SAM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>TLG</t>
+          <t>HUB</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>VJC</t>
+          <t>DVP</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>VHC</t>
+          <t>HSG</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>GEX</t>
+          <t>CEN</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CDC</t>
+          <t>HAR</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>GEE</t>
+          <t>CHS</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TNH</t>
+          <t>CMS</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TDT</t>
+          <t>TCO</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PAC</t>
+          <t>PRT</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SSH</t>
+          <t>PGB</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ACG</t>
+          <t>BTS</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DCS</t>
+          <t>SWC</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TDH</t>
+          <t>HNM</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>KHP</t>
+          <t>TAR</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>SRA</t>
+          <t>HIO</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TEG</t>
+          <t>PAS</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>STH</t>
+          <t>LHC</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SGR</t>
+          <t>CII</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SPI</t>
+          <t>TIP</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>VSH</t>
+          <t>PSH</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>VFS</t>
+          <t>HKB</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>HCD</t>
+          <t>PSD</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>VNA</t>
+          <t>VEA</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>KDM</t>
+          <t>TSA</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CLX</t>
+          <t>MCM</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>DIC</t>
+          <t>DGC</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>VCI</t>
+          <t>CDC</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>VOC</t>
+          <t>AAH</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>QTP</t>
+          <t>CRC</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>HSV</t>
+          <t>HAC</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PDR</t>
+          <t>CCL</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BVS</t>
+          <t>SBG</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CNG</t>
+          <t>PAT</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>ATG</t>
+          <t>FID</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>LTG</t>
+          <t>NAB</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>SWC</t>
+          <t>AAS</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>LHC</t>
+          <t>BGE</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>VIC</t>
+          <t>PDV</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>TVD</t>
+          <t>SBA</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>SBB</t>
+          <t>DLG</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>NXT</t>
+          <t>DVN</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>DPM</t>
+          <t>SDA</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>HQC</t>
+          <t>TIS</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MTA</t>
+          <t>TCW</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>PVS</t>
+          <t>LCG</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>FTM</t>
+          <t>ITC</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>ITQ</t>
+          <t>ITS</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BCE</t>
+          <t>SSB</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BCC</t>
+          <t>VLC</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>PVV</t>
+          <t>BCE</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>SVT</t>
+          <t>BMC</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BTN</t>
+          <t>BOT</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>THD</t>
+          <t>NDX</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>NVB</t>
+          <t>APG</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>PDV</t>
+          <t>PGI</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>HKB</t>
+          <t>MSB</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>D2D</t>
+          <t>NSH</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>TTH</t>
+          <t>HOM</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>FCN</t>
+          <t>TLH</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>PSP</t>
+          <t>PAC</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>BMC</t>
+          <t>QBS</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>NAG</t>
+          <t>TTA</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MPT</t>
+          <t>LTG</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>SBV</t>
+          <t>PLP</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>DTA</t>
+          <t>CTS</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CTG</t>
+          <t>CKG</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>HIO</t>
+          <t>VNE</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>GPC</t>
+          <t>TCH</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>BTP</t>
+          <t>HCD</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>AMV</t>
+          <t>VAB</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>HAG</t>
+          <t>PVR</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>DGC</t>
+          <t>VGT</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>FTS</t>
+          <t>THD</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>PVC</t>
+          <t>SCG</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>TNG</t>
+          <t>DID</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>NHV</t>
+          <t>TNS</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>AST</t>
+          <t>PGT</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>TCD</t>
+          <t>SDP</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>C69</t>
+          <t>IDJ</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>CTD</t>
+          <t>VDS</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>VKC</t>
+          <t>VID</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>PDB</t>
+          <t>PVD</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>PVD</t>
+          <t>TMS</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>VEC</t>
+          <t>MPT</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>SRB</t>
+          <t>XMC</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>GSP</t>
+          <t>PBP</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>VTO</t>
+          <t>GEG</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>TLD</t>
+          <t>PTL</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>DPR</t>
+          <t>SGR</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>TPB</t>
+          <t>SSN</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>SGT</t>
+          <t>LCM</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>NTC</t>
+          <t>PGS</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>NO1</t>
+          <t>DRI</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>FOC</t>
+          <t>TA9</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>POS</t>
+          <t>DCS</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>ACV</t>
+          <t>SZL</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>TLH</t>
+          <t>NAF</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>VGS</t>
+          <t>TDT</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>NHA</t>
+          <t>VPH</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>PCH</t>
+          <t>TVN</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>CCL</t>
+          <t>DXG</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>PGT</t>
+          <t>PSW</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>DBC</t>
+          <t>APC</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>PLP</t>
+          <t>DHA</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>AAS</t>
+          <t>MWG</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>STB</t>
+          <t>LPT</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>DBD</t>
+          <t>EIN</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>ABI</t>
+          <t>VNA</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>VNG</t>
+          <t>HDG</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LCG</t>
+          <t>DGW</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>PWA</t>
+          <t>HT1</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>PXL</t>
+          <t>TNH</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>DRI</t>
+          <t>PFL</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>SDD</t>
+          <t>VPB</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>FPT</t>
+          <t>PVP</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>VNR</t>
+          <t>SGI</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>HAC</t>
+          <t>HPG</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MIG</t>
+          <t>PXT</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>VTD</t>
+          <t>CTR</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>DXV</t>
+          <t>UDJ</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>REE</t>
+          <t>TAL</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>SFG</t>
+          <t>VTP</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>TDP</t>
+          <t>TRC</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>PXS</t>
+          <t>DBC</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>KDC</t>
+          <t>TDH</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>KHG</t>
+          <t>IVS</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>DVM</t>
+          <t>SBT</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>DHC</t>
+          <t>SGT</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>EVS</t>
+          <t>NHA</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>APH</t>
+          <t>BAF</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>PBP</t>
+          <t>BSI</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>BIG</t>
+          <t>HTP</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>KBC</t>
+          <t>VIX</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>VCB</t>
+          <t>HTI</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>HAX</t>
+          <t>MST</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>CIG</t>
+          <t>PVB</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>TVB</t>
+          <t>NCT</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>DPG</t>
+          <t>DC4</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>PC1</t>
+          <t>TL4</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>NBB</t>
+          <t>VHM</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>AMS</t>
+          <t>SD3</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>SZC</t>
+          <t>DFF</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>BNA</t>
+          <t>VLB</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>MCO</t>
+          <t>SGB</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>MPC</t>
+          <t>SJE</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>PSH</t>
+          <t>TCM</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>ORS</t>
+          <t>VC9</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>SCI</t>
+          <t>TNI</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>NCG</t>
+          <t>VCI</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>DDG</t>
+          <t>BSR</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>MWG</t>
+          <t>TV2</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>SDA</t>
+          <t>PTC</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>MSB</t>
+          <t>DTE</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>BOT</t>
+          <t>VNL</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>DDN</t>
+          <t>VIB</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>SBG</t>
+          <t>KKC</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>ILA</t>
+          <t>AGG</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>TMT</t>
+          <t>VHE</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>VTR</t>
+          <t>EVF</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>TCI</t>
+          <t>PVG</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>RIC</t>
+          <t>NBB</t>
         </is>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>DHG</t>
+          <t>TCL</t>
         </is>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>DTE</t>
+          <t>HD6</t>
         </is>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>MBB</t>
+          <t>C4G</t>
         </is>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>C47</t>
+          <t>BTP</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>KPF</t>
+          <t>TVB</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>CMG</t>
+          <t>SBS</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>PVB</t>
+          <t>PCH</t>
         </is>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>SDT</t>
+          <t>GIL</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>PHR</t>
+          <t>PC1</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>MAC</t>
+          <t>SD9</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>UDJ</t>
+          <t>BMS</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>EVE</t>
+          <t>VRE</t>
         </is>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>IDC</t>
+          <t>HDA</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>HLD</t>
+          <t>SCJ</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>FIR</t>
+          <t>SDD</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>LHG</t>
+          <t>POW</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>VNP</t>
+          <t>MHC</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>SMC</t>
+          <t>ACV</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>TDC</t>
+          <t>PVS</t>
         </is>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>OIL</t>
+          <t>G36</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>VHE</t>
+          <t>ACB</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>TIS</t>
+          <t>SKG</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>PVM</t>
+          <t>APS</t>
         </is>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>NT2</t>
+          <t>LGL</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>OCH</t>
+          <t>KHP</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>SHA</t>
+          <t>DTA</t>
         </is>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>TCB</t>
+          <t>PIV</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>SJS</t>
+          <t>MPC</t>
         </is>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>CTI</t>
+          <t>ANV</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>VCS</t>
+          <t>HDB</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>DID</t>
+          <t>PPC</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>DSE</t>
+          <t>STH</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>DVN</t>
+          <t>NT2</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>MCH</t>
+          <t>MZG</t>
         </is>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>TTF</t>
+          <t>VNH</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>BSI</t>
+          <t>POS</t>
         </is>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>PIV</t>
+          <t>WSS</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>VC7</t>
+          <t>VNM</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>BCA</t>
+          <t>TTN</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>MLS</t>
+          <t>KDH</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>PVG</t>
+          <t>CSV</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>DHA</t>
+          <t>NXT</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>IDI</t>
+          <t>VCG</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>VNM</t>
+          <t>SGP</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>VC3</t>
+          <t>ASM</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>SKG</t>
+          <t>VGI</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>ABS</t>
+          <t>TTF</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>CMT</t>
+          <t>TIN</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>THG</t>
+          <t>CSI</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>ACC</t>
+          <t>KSF</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>POW</t>
+          <t>KMR</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>HD6</t>
+          <t>CDO</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>NDN</t>
+          <t>CGV</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>CKG</t>
+          <t>CRE</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>THT</t>
+          <t>SDT</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>HDA</t>
+          <t>LDP</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>SAM</t>
+          <t>SVN</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>CST</t>
+          <t>RIC</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>DLG</t>
+          <t>OCH</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>PPH</t>
+          <t>FTM</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>LDG</t>
+          <t>HTT</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>HMC</t>
+          <t>NTC</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>GVR</t>
+          <t>CMT</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>KMR</t>
+          <t>CTD</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>NVL</t>
+          <t>GHC</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>SCG</t>
+          <t>HDC</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>OGC</t>
+          <t>BAB</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>CVT</t>
+          <t>KGM</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>SJM</t>
+          <t>BVG</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>KGM</t>
+          <t>FRT</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>PNJ</t>
+          <t>VGC</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>DFF</t>
+          <t>BMI</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>OCB</t>
+          <t>ITQ</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>BDT</t>
+          <t>DVM</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>BVH</t>
+          <t>GAS</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>HPX</t>
+          <t>EVE</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>HUB</t>
+          <t>SHA</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>ACL</t>
+          <t>FCN</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>LIX</t>
+          <t>DPM</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>VNE</t>
+          <t>VIC</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>NLG</t>
+          <t>ORS</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>AAA</t>
+          <t>DPR</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>DHM</t>
+          <t>TTH</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>TID</t>
+          <t>BCG</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>IJC</t>
+          <t>VPD</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>RYG</t>
+          <t>KSB</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>HHP</t>
+          <t>GMD</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>MFS</t>
+          <t>VMC</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>HTG</t>
+          <t>NO1</t>
         </is>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>HPG</t>
+          <t>VSC</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>JVC</t>
+          <t>LCS</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>VIT</t>
+          <t>L12</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>PSB</t>
+          <t>MCH</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>SGP</t>
+          <t>BCR</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>DGW</t>
+          <t>VOS</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>TAR</t>
+          <t>HAH</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>HNG</t>
+          <t>VHC</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>PVL</t>
+          <t>BCC</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>LGL</t>
+          <t>PGN</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>CTF</t>
+          <t>VTD</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>ADS</t>
+          <t>PVI</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>VE9</t>
+          <t>VRG</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>VAB</t>
+          <t>L14</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>VEA</t>
+          <t>NVL</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>DNM</t>
+          <t>DBT</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>HUT</t>
+          <t>SIP</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>BCR</t>
+          <t>PWA</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>SD6</t>
+          <t>VIT</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>VGI</t>
+          <t>ABW</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>HHG</t>
+          <t>HMC</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>VST</t>
+          <t>CTG</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>IPA</t>
+          <t>FIR</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>HID</t>
+          <t>HTG</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>DQC</t>
+          <t>HLD</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>DS3</t>
+          <t>VSH</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>HSG</t>
+          <t>GPC</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>AGG</t>
+          <t>ABB</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>KSB</t>
+          <t>SVT</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>CDO</t>
+          <t>D2D</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>SZL</t>
+          <t>DGT</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>HDB</t>
+          <t>GSP</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>TNI</t>
+          <t>VNG</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>VTK</t>
+          <t>VNB</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>VGC</t>
+          <t>TIG</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>DSC</t>
+          <t>VLG</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>VTZ</t>
+          <t>SMT</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>LSS</t>
+          <t>SD6</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>CEO</t>
+          <t>VC7</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>GMH</t>
+          <t>DCM</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>BMP</t>
+          <t>UDC</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>KOS</t>
+          <t>THG</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>SHS</t>
+          <t>CVT</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>BCM</t>
+          <t>MLS</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>DXS</t>
+          <t>AMS</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>VIB</t>
+          <t>VUA</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>TCL</t>
+          <t>KOS</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>NDX</t>
+          <t>STB</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>CHS</t>
+          <t>L18</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>CTP</t>
+          <t>VGG</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>VC9</t>
+          <t>DDV</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>UDC</t>
+          <t>TPB</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>HBC</t>
+          <t>DRC</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>VCG</t>
+          <t>PVT</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>BSR</t>
+          <t>VRC</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>PAS</t>
+          <t>HBC</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>APC</t>
+          <t>AGM</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>PAT</t>
+          <t>PTB</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>VNB</t>
+          <t>VTK</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>TVC</t>
+          <t>BTN</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>SGB</t>
+          <t>MBS</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>DXP</t>
+          <t>VPI</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>PBC</t>
+          <t>CSC</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>HOM</t>
+          <t>SAB</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>SHB</t>
+          <t>BMP</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>SDP</t>
+          <t>PVX</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>ITS</t>
+          <t>VND</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>VFG</t>
+          <t>OGC</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>DIG</t>
+          <t>NTP</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>TDM</t>
+          <t>LHG</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>MSR</t>
+          <t>DXV</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>DCM</t>
+          <t>PGV</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>GAS</t>
+          <t>SRA</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>LCS</t>
+          <t>NTL</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>VTV</t>
+          <t>PSI</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>GHC</t>
+          <t>NNC</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>BAF</t>
+          <t>TCI</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>PSW</t>
+          <t>ST8</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>VOS</t>
+          <t>VIG</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>ABW</t>
+          <t>VCB</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>PCG</t>
+          <t>DSE</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>NCT</t>
+          <t>DS3</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>QBS</t>
+          <t>BVB</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>LIG</t>
+          <t>PSP</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>BII</t>
+          <t>DHG</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>VMC</t>
+          <t>PXL</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>DCL</t>
+          <t>BID</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>BVB</t>
+          <t>KLB</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>KSF</t>
+          <t>CTF</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>DGT</t>
+          <t>HAP</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>TAL</t>
+          <t>SBB</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>BGE</t>
+          <t>IPA</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>PMB</t>
+          <t>CAG</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>TXM</t>
+          <t>DXP</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>PGN</t>
+          <t>VMD</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>HDC</t>
+          <t>CLX</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>PSE</t>
+          <t>NHV</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>HAH</t>
+          <t>VCR</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>HNM</t>
+          <t>NHH</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>VDS</t>
+          <t>TSC</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>VND</t>
+          <t>BNA</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>VNS</t>
+          <t>GKM</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>PVP</t>
+          <t>TVC</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>VIG</t>
+          <t>BIC</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>ABB</t>
+          <t>MFS</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>DTI</t>
+          <t>HIG</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>GDT</t>
+          <t>DVG</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>AAT</t>
+          <t>MCG</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>SGI</t>
+          <t>ATG</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>SHN</t>
+          <t>PXI</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>PPC</t>
+          <t>SJM</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>AFX</t>
+          <t>IDI</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>HVH</t>
+          <t>LSS</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>HIG</t>
+          <t>TDP</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>TV3</t>
+          <t>ADG</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>SD9</t>
+          <t>SCL</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>SD5</t>
+          <t>ACM</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>PSD</t>
+          <t>V21</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>XMC</t>
+          <t>DHC</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>VC1</t>
+          <t>TNG</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>HAP</t>
+          <t>HHS</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>VCS</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>VPG</t>
+          <t>HVN</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>NAF</t>
+          <t>DDG</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>TIP</t>
+          <t>MVC</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>ASM</t>
+          <t>KBC</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>SSN</t>
+          <t>SD5</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>BIC</t>
+          <t>VTZ</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>HSL</t>
+          <t>DSC</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>PGI</t>
+          <t>EIB</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>SCJ</t>
+          <t>HVH</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>PVC</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>DTD</t>
+          <t>ASP</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>HVN</t>
+          <t>BCM</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>TCW</t>
+          <t>DTD</t>
         </is>
       </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>PLC</t>
+          <t>VFG</t>
         </is>
       </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>BCG</t>
+          <t>DST</t>
         </is>
       </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>CRE</t>
+          <t>PET</t>
         </is>
       </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>GIL</t>
+          <t>C69</t>
         </is>
       </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>GKM</t>
+          <t>HNG</t>
         </is>
       </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>PRE</t>
+          <t>HHG</t>
         </is>
       </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>AGM</t>
+          <t>QNC</t>
         </is>
       </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>SCR</t>
+          <t>C32</t>
         </is>
       </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>DMC</t>
+          <t>PNJ</t>
         </is>
       </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>HTI</t>
+          <t>HTN</t>
         </is>
       </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>QNC</t>
+          <t>NRC</t>
         </is>
       </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>VLC</t>
+          <t>CTI</t>
         </is>
       </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>DDV</t>
+          <t>HU4</t>
         </is>
       </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>BMI</t>
+          <t>ABI</t>
         </is>
       </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>L14</t>
+          <t>ILA</t>
         </is>
       </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>FCM</t>
+          <t>SVD</t>
         </is>
       </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>HDG</t>
+          <t>ACG</t>
         </is>
       </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>SBA</t>
+          <t>MTA</t>
         </is>
       </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>PTC</t>
+          <t>HND</t>
         </is>
       </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>ASP</t>
+          <t>DHM</t>
         </is>
       </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>SCL</t>
+          <t>VGS</t>
         </is>
       </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>GIC</t>
+          <t>SSI</t>
         </is>
       </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>NHH</t>
+          <t>OCB</t>
         </is>
       </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>APS</t>
+          <t>HVA</t>
         </is>
       </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>V21</t>
+          <t>GDT</t>
         </is>
       </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>SBT</t>
+          <t>SMC</t>
         </is>
       </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>DST</t>
+          <t>BIG</t>
         </is>
       </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>VCR</t>
+          <t>NCG</t>
         </is>
       </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>PPT</t>
+          <t>HHP</t>
         </is>
       </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>ACB</t>
+          <t>QCG</t>
         </is>
       </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>HTP</t>
+          <t>BII</t>
         </is>
       </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>PVI</t>
+          <t>TNT</t>
         </is>
       </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>QNS</t>
+          <t>FOC</t>
         </is>
       </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>API</t>
+          <t>HTM</t>
         </is>
       </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>BVG</t>
+          <t>PBC</t>
         </is>
       </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>VSC</t>
+          <t>PVV</t>
         </is>
       </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>NDT</t>
+          <t>API</t>
         </is>
       </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>SJE</t>
+          <t>KHG</t>
         </is>
       </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>LPB</t>
+          <t>DTI</t>
         </is>
       </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>ICT</t>
+          <t>RYG</t>
         </is>
       </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>TNS</t>
+          <t>GIC</t>
         </is>
       </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>IDJ</t>
+          <t>SHS</t>
         </is>
       </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>HT1</t>
+          <t>VHG</t>
         </is>
       </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>EIN</t>
+          <t>FIT</t>
         </is>
       </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>FIT</t>
+          <t>TYA</t>
         </is>
       </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>C4G</t>
+          <t>TDC</t>
         </is>
       </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>VRE</t>
+          <t>GMH</t>
         </is>
       </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>DC4</t>
+          <t>TVD</t>
         </is>
       </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>SSB</t>
+          <t>NDN</t>
         </is>
       </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>CRC</t>
+          <t>BWE</t>
         </is>
       </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>SBS</t>
+          <t>AFX</t>
         </is>
       </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>AGR</t>
+          <t>JVC</t>
         </is>
       </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>MBG</t>
+          <t>DDN</t>
         </is>
       </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>PFL</t>
+          <t>HSL</t>
         </is>
       </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>PVO</t>
+          <t>NKG</t>
         </is>
       </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>HAR</t>
+          <t>TCD</t>
         </is>
       </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>TSA</t>
+          <t>NVB</t>
         </is>
       </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>SCS</t>
+          <t>NED</t>
         </is>
       </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>PXI</t>
+          <t>SZC</t>
         </is>
       </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>SMT</t>
+          <t>VIP</t>
         </is>
       </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>TTA</t>
+          <t>DIG</t>
         </is>
       </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>PHC</t>
+          <t>AGR</t>
         </is>
       </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>BTS</t>
+          <t>VJC</t>
         </is>
       </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>KKC</t>
+          <t>MSR</t>
         </is>
       </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>TVS</t>
+          <t>PSB</t>
         </is>
       </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>VNL</t>
+          <t>GEX</t>
         </is>
       </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>VPB</t>
+          <t>THT</t>
         </is>
       </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>PVR</t>
+          <t>CST</t>
         </is>
       </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>TYA</t>
+          <t>VST</t>
         </is>
       </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>HCM</t>
         </is>
       </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>PHP</t>
+          <t>HPX</t>
         </is>
       </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>WSS</t>
+          <t>S99</t>
         </is>
       </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>VUA</t>
+          <t>LPB</t>
         </is>
       </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>VIP</t>
+          <t>ABC</t>
         </is>
       </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>VRC</t>
+          <t>FCM</t>
         </is>
       </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>VLB</t>
+          <t>KDM</t>
         </is>
       </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>VC2</t>
+          <t>PDR</t>
         </is>
       </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>C32</t>
+          <t>NAG</t>
         </is>
       </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>MHC</t>
+          <t>IMP</t>
         </is>
       </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>HTT</t>
+          <t>C47</t>
         </is>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>AAH</t>
+          <t>MSH</t>
         </is>
       </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>ST8</t>
+          <t>PSE</t>
         </is>
       </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>VIX</t>
+          <t>VTO</t>
         </is>
       </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>VHG</t>
+          <t>BCA</t>
         </is>
       </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>KSD</t>
+          <t>CTP</t>
         </is>
       </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>PVX</t>
+          <t>GEE</t>
         </is>
       </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>KVC</t>
+          <t>PCG</t>
         </is>
       </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>CSC</t>
+          <t>VTR</t>
         </is>
       </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>CSI</t>
+          <t>PVO</t>
         </is>
       </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>FID</t>
+          <t>FMC</t>
         </is>
       </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>PGV</t>
+          <t>EVG</t>
         </is>
       </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>HCM</t>
+          <t>IDC</t>
         </is>
       </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>ELC</t>
+          <t>SHN</t>
         </is>
       </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>FOX</t>
+          <t>NBC</t>
         </is>
       </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>VPI</t>
+          <t>DNM</t>
         </is>
       </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>HVA</t>
+          <t>SJS</t>
         </is>
       </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
         <is>
-          <t>QCG</t>
+          <t>MBB</t>
         </is>
       </c>
     </row>
     <row r="492">
       <c r="A492" t="inlineStr">
         <is>
-          <t>SHI</t>
+          <t>BVS</t>
         </is>
       </c>
     </row>
     <row r="493">
       <c r="A493" t="inlineStr">
         <is>
-          <t>PVT</t>
+          <t>VC3</t>
         </is>
       </c>
     </row>
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>TSC</t>
+          <t>TV3</t>
         </is>
       </c>
     </row>
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>PLX</t>
+          <t>MIG</t>
         </is>
       </c>
     </row>
     <row r="496">
       <c r="A496" t="inlineStr">
         <is>
-          <t>NRC</t>
+          <t>MAC</t>
         </is>
       </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
         <is>
-          <t>EVF</t>
+          <t>HII</t>
         </is>
       </c>
     </row>
     <row r="498">
       <c r="A498" t="inlineStr">
         <is>
-          <t>PET</t>
+          <t>VC2</t>
         </is>
       </c>
     </row>
     <row r="499">
       <c r="A499" t="inlineStr">
         <is>
-          <t>MSH</t>
+          <t>KSQ</t>
         </is>
       </c>
     </row>
     <row r="500">
       <c r="A500" t="inlineStr">
         <is>
-          <t>LPT</t>
+          <t>AST</t>
         </is>
       </c>
     </row>
     <row r="501">
       <c r="A501" t="inlineStr">
         <is>
-          <t>VGT</t>
+          <t>PAN</t>
         </is>
       </c>
     </row>
     <row r="502">
       <c r="A502" t="inlineStr">
         <is>
-          <t>SAB</t>
+          <t>PHR</t>
         </is>
       </c>
     </row>
     <row r="503">
       <c r="A503" t="inlineStr">
         <is>
-          <t>HTN</t>
+          <t>NVT</t>
         </is>
       </c>
     </row>
     <row r="504">
       <c r="A504" t="inlineStr">
         <is>
-          <t>CGV</t>
+          <t>CMX</t>
         </is>
       </c>
     </row>
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>ADG</t>
+          <t>PRE</t>
         </is>
       </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>VMD</t>
+          <t>HBS</t>
         </is>
       </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
         <is>
-          <t>DVP</t>
+          <t>HAX</t>
         </is>
       </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
         <is>
-          <t>NED</t>
+          <t>ACL</t>
         </is>
       </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
         <is>
-          <t>TIN</t>
+          <t>VNR</t>
         </is>
       </c>
     </row>
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>CAG</t>
+          <t>PV2</t>
         </is>
       </c>
     </row>
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>NVT</t>
+          <t>KSD</t>
         </is>
       </c>
     </row>
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>MCM</t>
+          <t>LDG</t>
         </is>
       </c>
     </row>
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>MST</t>
+          <t>VFS</t>
         </is>
       </c>
     </row>
     <row r="514">
       <c r="A514" t="inlineStr">
         <is>
-          <t>NTL</t>
+          <t>AAV</t>
         </is>
       </c>
     </row>
     <row r="515">
       <c r="A515" t="inlineStr">
         <is>
-          <t>MCG</t>
+          <t>HQC</t>
         </is>
       </c>
     </row>
     <row r="516">
       <c r="A516" t="inlineStr">
         <is>
-          <t>VLG</t>
+          <t>SPI</t>
         </is>
       </c>
     </row>
     <row r="517">
       <c r="A517" t="inlineStr">
         <is>
-          <t>SIP</t>
+          <t>DIC</t>
         </is>
       </c>
     </row>
     <row r="518">
       <c r="A518" t="inlineStr">
         <is>
-          <t>CSV</t>
+          <t>PLX</t>
         </is>
       </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
         <is>
-          <t>YEG</t>
+          <t>SBV</t>
         </is>
       </c>
     </row>
     <row r="520">
       <c r="A520" t="inlineStr">
         <is>
-          <t>G36</t>
+          <t>LIG</t>
         </is>
       </c>
     </row>
     <row r="521">
       <c r="A521" t="inlineStr">
         <is>
-          <t>ABC</t>
+          <t>ODE</t>
         </is>
       </c>
     </row>
     <row r="522">
       <c r="A522" t="inlineStr">
         <is>
-          <t>NSH</t>
+          <t>DCL</t>
         </is>
       </c>
     </row>
     <row r="523">
       <c r="A523" t="inlineStr">
         <is>
-          <t>IVS</t>
+          <t>TEG</t>
         </is>
       </c>
     </row>
     <row r="524">
       <c r="A524" t="inlineStr">
         <is>
-          <t>VSE</t>
+          <t>QTP</t>
         </is>
       </c>
     </row>
     <row r="525">
       <c r="A525" t="inlineStr">
         <is>
-          <t>VCC</t>
+          <t>PLC</t>
         </is>
       </c>
     </row>
     <row r="526">
       <c r="A526" t="inlineStr">
         <is>
-          <t>HBS</t>
+          <t>VOC</t>
         </is>
       </c>
     </row>
     <row r="527">
       <c r="A527" t="inlineStr">
         <is>
-          <t>APG</t>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>TTN</t>
+          <t>SJD</t>
         </is>
       </c>
     </row>
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>TRC</t>
+          <t>TDG</t>
         </is>
       </c>
     </row>
     <row r="530">
       <c r="A530" t="inlineStr">
         <is>
-          <t>ACM</t>
+          <t>PGC</t>
         </is>
       </c>
     </row>
     <row r="531">
       <c r="A531" t="inlineStr">
         <is>
-          <t>KSQ</t>
+          <t>DL1</t>
         </is>
       </c>
     </row>
     <row r="532">
       <c r="A532" t="inlineStr">
         <is>
-          <t>HHV</t>
+          <t>DPG</t>
         </is>
       </c>
     </row>
     <row r="533">
       <c r="A533" t="inlineStr">
         <is>
-          <t>DRC</t>
+          <t>TCB</t>
         </is>
       </c>
     </row>
     <row r="534">
       <c r="A534" t="inlineStr">
         <is>
-          <t>NAB</t>
+          <t>ABS</t>
         </is>
       </c>
     </row>
     <row r="535">
       <c r="A535" t="inlineStr">
         <is>
-          <t>VPH</t>
+          <t>LMH</t>
         </is>
       </c>
     </row>
     <row r="536">
       <c r="A536" t="inlineStr">
         <is>
-          <t>GDA</t>
+          <t>KDC</t>
         </is>
       </c>
     </row>
     <row r="537">
       <c r="A537" t="inlineStr">
         <is>
-          <t>PGC</t>
+          <t>NDT</t>
         </is>
       </c>
     </row>
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t>BWE</t>
+          <t>ILB</t>
         </is>
       </c>
     </row>
     <row r="539">
       <c r="A539" t="inlineStr">
         <is>
-          <t>LAS</t>
+          <t>BFC</t>
         </is>
       </c>
     </row>
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>HU4</t>
+          <t>BVH</t>
         </is>
       </c>
     </row>
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>GMD</t>
+          <t>VC1</t>
         </is>
       </c>
     </row>
     <row r="542">
       <c r="A542" t="inlineStr">
         <is>
-          <t>AAV</t>
+          <t>YEG</t>
         </is>
       </c>
     </row>
     <row r="543">
       <c r="A543" t="inlineStr">
         <is>
-          <t>BFC</t>
+          <t>TVS</t>
         </is>
       </c>
     </row>
     <row r="544">
       <c r="A544" t="inlineStr">
         <is>
-          <t>ITD</t>
+          <t>VNP</t>
         </is>
       </c>
     </row>
     <row r="545">
       <c r="A545" t="inlineStr">
         <is>
-          <t>HMR</t>
+          <t>VEC</t>
         </is>
       </c>
     </row>
     <row r="546">
       <c r="A546" t="inlineStr">
         <is>
-          <t>TL4</t>
+          <t>PPT</t>
         </is>
       </c>
     </row>
     <row r="547">
       <c r="A547" t="inlineStr">
         <is>
-          <t>FRT</t>
+          <t>TLD</t>
         </is>
       </c>
     </row>
     <row r="548">
       <c r="A548" t="inlineStr">
         <is>
-          <t>PV2</t>
+          <t>OIL</t>
         </is>
       </c>
     </row>
     <row r="549">
       <c r="A549" t="inlineStr">
         <is>
-          <t>VID</t>
+          <t>VKC</t>
         </is>
       </c>
     </row>
     <row r="550">
       <c r="A550" t="inlineStr">
         <is>
-          <t>L18</t>
+          <t>TDM</t>
         </is>
       </c>
     </row>
     <row r="551">
       <c r="A551" t="inlineStr">
         <is>
-          <t>SSI</t>
+          <t>FTS</t>
         </is>
       </c>
     </row>
     <row r="552">
       <c r="A552" t="inlineStr">
         <is>
-          <t>TDG</t>
+          <t>EVS</t>
         </is>
       </c>
     </row>
     <row r="553">
       <c r="A553" t="inlineStr">
         <is>
-          <t>TA9</t>
+          <t>CIG</t>
         </is>
       </c>
     </row>
     <row r="554">
       <c r="A554" t="inlineStr">
         <is>
-          <t>PSI</t>
+          <t>SHI</t>
         </is>
       </c>
     </row>
     <row r="555">
       <c r="A555" t="inlineStr">
         <is>
-          <t>PTL</t>
+          <t>ELC</t>
         </is>
       </c>
     </row>
     <row r="556">
       <c r="A556" t="inlineStr">
         <is>
-          <t>NTP</t>
+          <t>REE</t>
         </is>
       </c>
     </row>
     <row r="557">
       <c r="A557" t="inlineStr">
         <is>
-          <t>LMH</t>
+          <t>DBD</t>
         </is>
       </c>
     </row>
     <row r="558">
       <c r="A558" t="inlineStr">
         <is>
-          <t>EIB</t>
+          <t>HVX</t>
         </is>
       </c>
     </row>
     <row r="559">
       <c r="A559" t="inlineStr">
         <is>
-          <t>SJD</t>
+          <t>TID</t>
         </is>
       </c>
     </row>
     <row r="560">
       <c r="A560" t="inlineStr">
         <is>
-          <t>PTB</t>
+          <t>SRB</t>
         </is>
       </c>
     </row>
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>HII</t>
+          <t>ACC</t>
         </is>
       </c>
     </row>
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>NKG</t>
+          <t>GDA</t>
         </is>
       </c>
     </row>
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>PXT</t>
+          <t>GVR</t>
         </is>
       </c>
     </row>
     <row r="564">
       <c r="A564" t="inlineStr">
         <is>
-          <t>BAB</t>
+          <t>AAT</t>
         </is>
       </c>
     </row>
     <row r="565">
       <c r="A565" t="inlineStr">
         <is>
-          <t>SVD</t>
+          <t>STK</t>
         </is>
       </c>
     </row>
     <row r="566">
       <c r="A566" t="inlineStr">
         <is>
-          <t>POM</t>
+          <t>KPF</t>
         </is>
       </c>
     </row>
     <row r="567">
       <c r="A567" t="inlineStr">
         <is>
-          <t>LDP</t>
+          <t>HAG</t>
         </is>
       </c>
     </row>
     <row r="568">
       <c r="A568" t="inlineStr">
         <is>
-          <t>CMS</t>
+          <t>PVL</t>
         </is>
       </c>
     </row>
     <row r="569">
       <c r="A569" t="inlineStr">
         <is>
-          <t>VPD</t>
+          <t>IJC</t>
         </is>
       </c>
     </row>
     <row r="570">
       <c r="A570" t="inlineStr">
         <is>
-          <t>VNH</t>
+          <t>TMT</t>
         </is>
       </c>
     </row>
     <row r="571">
       <c r="A571" t="inlineStr">
         <is>
-          <t>TCH</t>
+          <t>BDT</t>
         </is>
       </c>
     </row>
     <row r="572">
       <c r="A572" t="inlineStr">
         <is>
-          <t>BMS</t>
+          <t>PMB</t>
         </is>
       </c>
     </row>
     <row r="573">
       <c r="A573" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>HID</t>
         </is>
       </c>
     </row>
     <row r="574">
       <c r="A574" t="inlineStr">
         <is>
-          <t>NNC</t>
+          <t>PDB</t>
         </is>
       </c>
     </row>
     <row r="575">
       <c r="A575" t="inlineStr">
         <is>
-          <t>DL1</t>
+          <t>KVC</t>
         </is>
       </c>
     </row>
     <row r="576">
       <c r="A576" t="inlineStr">
         <is>
-          <t>DAH</t>
+          <t>PHP</t>
         </is>
       </c>
     </row>
     <row r="577">
       <c r="A577" t="inlineStr">
         <is>
-          <t>SD3</t>
+          <t>HMR</t>
         </is>
       </c>
     </row>
     <row r="578">
       <c r="A578" t="inlineStr">
         <is>
-          <t>FMC</t>
+          <t>VNS</t>
         </is>
       </c>
     </row>
     <row r="579">
       <c r="A579" t="inlineStr">
         <is>
-          <t>CII</t>
+          <t>FPT</t>
         </is>
       </c>
     </row>
     <row r="580">
       <c r="A580" t="inlineStr">
         <is>
-          <t>KLB</t>
+          <t>DXS</t>
         </is>
       </c>
     </row>
     <row r="581">
       <c r="A581" t="inlineStr">
         <is>
-          <t>HHS</t>
+          <t>HUT</t>
         </is>
       </c>
     </row>
     <row r="582">
       <c r="A582" t="inlineStr">
         <is>
-          <t>TIG</t>
+          <t>SCR</t>
         </is>
       </c>
     </row>
     <row r="583">
       <c r="A583" t="inlineStr">
         <is>
-          <t>GEG</t>
+          <t>HHV</t>
         </is>
       </c>
     </row>
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>TVN</t>
+          <t>CMG</t>
         </is>
       </c>
     </row>
     <row r="585">
       <c r="A585" t="inlineStr">
         <is>
-          <t>VGG</t>
+          <t>AAA</t>
         </is>
       </c>
     </row>
     <row r="586">
       <c r="A586" t="inlineStr">
         <is>
-          <t>ILB</t>
+          <t>VPG</t>
         </is>
       </c>
     </row>
     <row r="587">
       <c r="A587" t="inlineStr">
         <is>
-          <t>VBB</t>
+          <t>MBG</t>
         </is>
       </c>
     </row>
     <row r="588">
       <c r="A588" t="inlineStr">
         <is>
-          <t>HTM</t>
+          <t>AMV</t>
         </is>
       </c>
     </row>
     <row r="589">
       <c r="A589" t="inlineStr">
         <is>
-          <t>ANV</t>
+          <t>SFG</t>
         </is>
       </c>
     </row>
     <row r="590">
       <c r="A590" t="inlineStr">
         <is>
-          <t>BKG</t>
+          <t>VTV</t>
         </is>
       </c>
     </row>
     <row r="591">
       <c r="A591" t="inlineStr">
         <is>
-          <t>L12</t>
+          <t>CNG</t>
         </is>
       </c>
     </row>
     <row r="592">
       <c r="A592" t="inlineStr">
         <is>
-          <t>CTR</t>
+          <t>MCO</t>
         </is>
       </c>
     </row>
     <row r="593">
       <c r="A593" t="inlineStr">
         <is>
-          <t>TV2</t>
+          <t>DMC</t>
         </is>
       </c>
     </row>
     <row r="594">
       <c r="A594" t="inlineStr">
         <is>
-          <t>HVX</t>
+          <t>DAH</t>
         </is>
       </c>
     </row>
     <row r="595">
       <c r="A595" t="inlineStr">
         <is>
-          <t>BID</t>
+          <t>QNS</t>
         </is>
       </c>
     </row>
     <row r="596">
       <c r="A596" t="inlineStr">
         <is>
-          <t>VRG</t>
+          <t>ICT</t>
         </is>
       </c>
     </row>
     <row r="597">
       <c r="A597" t="inlineStr">
         <is>
-          <t>S99</t>
+          <t>HSV</t>
         </is>
       </c>
     </row>
     <row r="598">
       <c r="A598" t="inlineStr">
         <is>
-          <t>DVG</t>
+          <t>VBB</t>
         </is>
       </c>
     </row>
     <row r="599">
       <c r="A599" t="inlineStr">
         <is>
-          <t>MBS</t>
+          <t>POM</t>
         </is>
       </c>
     </row>
     <row r="600">
       <c r="A600" t="inlineStr">
         <is>
-          <t>IMP</t>
+          <t>TLG</t>
         </is>
       </c>
     </row>
     <row r="601">
       <c r="A601" t="inlineStr">
         <is>
-          <t>MSN</t>
+          <t>ITD</t>
         </is>
       </c>
     </row>
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>CTS</t>
+          <t>DHT</t>
         </is>
       </c>
     </row>
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>VTP</t>
+          <t>TXM</t>
         </is>
       </c>
     </row>
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>SSH</t>
         </is>
       </c>
     </row>
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>SAV</t>
+          <t>SCS</t>
         </is>
       </c>
     </row>
     <row r="606">
       <c r="A606" t="inlineStr">
         <is>
-          <t>EVG</t>
+          <t>PPH</t>
         </is>
       </c>
     </row>
     <row r="607">
       <c r="A607" t="inlineStr">
         <is>
-          <t>ODE</t>
+          <t>SCI</t>
         </is>
       </c>
     </row>
     <row r="608">
       <c r="A608" t="inlineStr">
         <is>
-          <t>DBT</t>
+          <t>CEO</t>
         </is>
       </c>
     </row>
     <row r="609">
       <c r="A609" t="inlineStr">
         <is>
-          <t>TCO</t>
+          <t>CSM</t>
         </is>
       </c>
     </row>
     <row r="610">
       <c r="A610" t="inlineStr">
         <is>
-          <t>LCM</t>
+          <t>MSN</t>
         </is>
       </c>
     </row>
     <row r="611">
       <c r="A611" t="inlineStr">
         <is>
-          <t>PGS</t>
+          <t>BKG</t>
         </is>
       </c>
     </row>
     <row r="612">
       <c r="A612" t="inlineStr">
         <is>
-          <t>MZG</t>
+          <t>VSE</t>
         </is>
       </c>
     </row>
     <row r="613">
       <c r="A613" t="inlineStr">
         <is>
-          <t>CSM</t>
+          <t>APH</t>
         </is>
       </c>
     </row>
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>TCM</t>
+          <t>DQC</t>
         </is>
       </c>
     </row>
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>DXG</t>
+          <t>SAV</t>
         </is>
       </c>
     </row>
     <row r="616">
       <c r="A616" t="inlineStr">
         <is>
-          <t>DHT</t>
+          <t>SHB</t>
         </is>
       </c>
     </row>
     <row r="617">
       <c r="A617" t="inlineStr">
         <is>
-          <t>CEN</t>
+          <t>PHC</t>
         </is>
       </c>
     </row>
     <row r="618">
       <c r="A618" t="inlineStr">
         <is>
-          <t>VHM</t>
+          <t>PXS</t>
         </is>
       </c>
     </row>

</xml_diff>